<commit_message>
adjusted boards for validity
</commit_message>
<xml_diff>
--- a/ClueGame/data/ClueLayout.xlsx
+++ b/ClueGame/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazem\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijah/Desktop/Mines/Fall 2024/Software Engineering/Clue/ClueGame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04A4148B-C5FA-46D5-8975-4B6BC3EA7613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBD2F81-1E3F-F94D-9118-887D4E3723C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{650C51C9-D872-4760-9F9A-5F77CF585FAE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="13880" xr2:uid="{650C51C9-D872-4760-9F9A-5F77CF585FAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="34">
   <si>
     <t>L</t>
   </si>
@@ -567,16 +567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5735F3-DA52-47B7-A6B0-3EAA213C71FB}">
   <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="67" width="3.59765625" customWidth="1"/>
+    <col min="1" max="67" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B1" s="6">
         <v>0</v>
       </c>
@@ -680,7 +680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -787,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -894,7 +894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -3594,7 +3594,9 @@
       <c r="H29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J29" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Got all adjacency tests to pass
</commit_message>
<xml_diff>
--- a/ClueGame/data/ClueLayout.xlsx
+++ b/ClueGame/data/ClueLayout.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijah/Desktop/Mines/Fall 2024/Software Engineering/Clue/ClueGame/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBD2F81-1E3F-F94D-9118-887D4E3723C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{10566ECD-B95D-44E3-B320-0CB8F16AA8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="13880" xr2:uid="{650C51C9-D872-4760-9F9A-5F77CF585FAE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{650C51C9-D872-4760-9F9A-5F77CF585FAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -567,16 +563,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5735F3-DA52-47B7-A6B0-3EAA213C71FB}">
   <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="67" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B1" s="6">
         <v>0</v>
       </c>
@@ -680,7 +676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -787,7 +783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -894,7 +890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -1001,7 +997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -1108,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -1215,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -1322,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -1429,7 +1425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -1536,7 +1532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -1643,7 +1639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -1750,7 +1746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -1857,7 +1853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -1964,7 +1960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -2071,7 +2067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -2178,7 +2174,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -2285,7 +2281,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -2371,7 +2367,7 @@
         <v>6</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="AD17" s="3" t="s">
         <v>6</v>
@@ -2392,7 +2388,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -2499,7 +2495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -2606,7 +2602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -2713,7 +2709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -2820,7 +2816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -2927,7 +2923,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -3034,7 +3030,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -3141,7 +3137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -3248,7 +3244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -3355,7 +3351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -3462,7 +3458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -3569,7 +3565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
         <v>27</v>
       </c>

</xml_diff>